<commit_message>
Xóa các thư viện không cần và thay đổi code login
</commit_message>
<xml_diff>
--- a/target/classes/Data/Login.xlsx
+++ b/target/classes/Data/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\Java\src\JaVaTestAppium\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8F1843-1EEF-4E63-B874-1A4F072AA990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B963CD78-7415-4A11-BE5B-0813E48B5803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4236" yWindow="2244" windowWidth="17280" windowHeight="8964" xr2:uid="{F893E997-8251-44C5-9FC1-92383C03822B}"/>
   </bookViews>
@@ -33,15 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>user</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>nhuyyy@gmail.com</t>
-  </si>
-  <si>
-    <t>password</t>
   </si>
   <si>
     <t>phong@gmail.com</t>
@@ -415,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C39D2F2-F80F-494B-8407-2C45F22731E6}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A2:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -426,21 +420,13 @@
     <col min="1" max="16384" width="30.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
@@ -449,7 +435,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -459,15 +445,15 @@
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
         <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>3</v>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C7" s="1">
         <v>12345678</v>
@@ -475,12 +461,12 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{76059046-6809-4ED4-9CAB-EBF959530B69}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{76059046-6809-4ED4-9CAB-EBF959530B69}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>